<commit_message>
updated Surefire plugin and excel reader
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17070" windowHeight="2925"/>
   </bookViews>
   <sheets>
     <sheet name="SheetData" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -367,6 +368,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>